<commit_message>
added some more Question
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF931BEF-2F14-49F6-81DF-413773F15211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4FD36E-4492-4DF5-BFB4-40230EA92C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,24 @@
   </si>
   <si>
     <t>Day 4</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Day 6</t>
+  </si>
+  <si>
+    <t>Day 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 8 </t>
+  </si>
+  <si>
+    <t>Day 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 10 </t>
   </si>
 </sst>
 </file>
@@ -358,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,6 +423,57 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>